<commit_message>
Added shipping page and fixes for home and footer page.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/HomePageTestData.xlsx
+++ b/src/test/resources/TestData/HomePageTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SJI-GOA-70\Downloads\template-selenium-main\template-selenium-main\Neostrata\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadee\git\Neostrata\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E75699E-D06E-4CFA-8C76-D35C472AC0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36EA2830-A3AC-4847-A8EC-2A33156E4425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2256" yWindow="984" windowWidth="20784" windowHeight="11256" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logo" sheetId="10" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
   <si>
     <t>TestCase</t>
   </si>
@@ -80,13 +80,10 @@
     <t>products/high-potency-cream</t>
   </si>
   <si>
-    <t>products/rebound-sculpting-cream</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>index</t>
+  </si>
+  <si>
+    <t>products/hydra-filling-cream-2</t>
   </si>
 </sst>
 </file>
@@ -433,7 +430,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -458,7 +455,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -471,7 +468,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -496,7 +493,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -512,7 +509,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -541,7 +538,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -560,7 +557,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -585,7 +582,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -601,7 +598,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -623,7 +620,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -694,7 +691,7 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>